<commit_message>
adding surgery notes and physiology notes
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CH_061614_D.xlsx
+++ b/Mouse_workbooks/CH_061614_D.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Mouse_workbooks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="140" windowWidth="14740" windowHeight="16680" tabRatio="624"/>
+    <workbookView xWindow="1185" yWindow="135" windowWidth="14745" windowHeight="16680" tabRatio="624"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -130,9 +135,6 @@
     <t>EMX-Cre+/-</t>
   </si>
   <si>
-    <t xml:space="preserve">Injected AAV9.flexed.ChR2.tdTomato. </t>
-  </si>
-  <si>
     <t>CH_061614_D</t>
   </si>
   <si>
@@ -143,6 +145,63 @@
   </si>
   <si>
     <t>Injected 100 nl at 2.55 mm Left of lambda at a depth of 400 um. Injected AAV2/9.flexed.ChR2.tdTomato (addgene 18917).</t>
+  </si>
+  <si>
+    <t>K-Gluconate and Cs-Gluconate</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>299, 290</t>
+  </si>
+  <si>
+    <t>Recording from pairs of neurons, looking for connected pairs where the presynaptic neuron is an inhibitory neuon so that I can measure the reversal potential for Cl- using the Cs-Gluconate internal.</t>
+  </si>
+  <si>
+    <t>2014_07_09_0000</t>
+  </si>
+  <si>
+    <t>Paired recording. Presynaptic neuron is inhibitory. Both electrodes are filled with Cs-Gluconate. Holding potential for post-synaptic neuron was -40 mV.</t>
+  </si>
+  <si>
+    <t>2014_07_09_0001</t>
+  </si>
+  <si>
+    <t>1 sweep per holding potential for measuring reversal potential for chloride.</t>
+  </si>
+  <si>
+    <t>2014_07_09_0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 sweeps per run, measuring reversal potential. Very small post-synaptic currents, but measureable. </t>
+  </si>
+  <si>
+    <t>10 sweeps per run, measuring reversal potential. Very small post-synaptic currents, but measureable. This file is different than _0002 only in the respect that I applied a little negative pressure to the post-synptic cell to get better access to that cell. Slightly cleaner data than _0002</t>
+  </si>
+  <si>
+    <t>2014_07_09_0003</t>
+  </si>
+  <si>
+    <t>2014_07_09_0004</t>
+  </si>
+  <si>
+    <t>gap free in voltage clamp from both cells. The inhibitory neuron is on channel 2 and show very apparent rhythmic oscilations in membrane current. Cs internal in both cells and has been applied in the inhibitory cell for at least an hour. -60 mV holding potential for each cell.</t>
+  </si>
+  <si>
+    <t>file _0003 Vm</t>
+  </si>
+  <si>
+    <t>file _0003 Im</t>
+  </si>
+  <si>
+    <t>file _0002 Im</t>
+  </si>
+  <si>
+    <t>file _0002 Vm</t>
+  </si>
+  <si>
+    <t>Injected AAV9.flexed.ChR2.tdTomato. Whole cell recordings from connected pairs to estimate reversal potential for chloride using the new Cesium internal.</t>
   </si>
 </sst>
 </file>
@@ -797,6 +856,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -806,15 +889,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -905,6 +979,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -916,36 +1005,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -970,6 +1029,1901 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>IV curve from File  _0003</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Analysis!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-119.28594970703099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-107.45529937744099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-95.554893493652301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-83.666122436523395</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-71.812217712402301</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-59.924896240234297</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-48.044841766357401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Analysis!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-8.1960477828979403</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.9468455314636204</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.5849814414978001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.8713792562484699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.72266530990600597</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.64208555221557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.7224264144897408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="263807248"/>
+        <c:axId val="263803888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="263807248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="263803888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="263803888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="263807248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>IV</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> curve from File _0002</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.4011596675415573"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Analysis!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-119.276565551757</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-107.4468460083</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-95.544990539550696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-83.659782409667898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-71.810638427734304</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-59.928199768066399</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-48.055477142333899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Analysis!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-4.2161784172058097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.84029865264892</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.1803574562072701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.0234618186950599</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.33055078983306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.36196541786193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7743024826049796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="296231968"/>
+        <c:axId val="296239248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="296231968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296239248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="296239248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="296231968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1300,74 +3254,74 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="38" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="62.375" style="27" customWidth="1"/>
     <col min="3" max="16384" width="18.5" style="9" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38" customHeight="1" thickTop="1">
+    <row r="1" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="38" customHeight="1">
+      <c r="B1" s="28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38" customHeight="1">
+    <row r="3" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="30">
         <v>41782</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38" customHeight="1">
+    <row r="4" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38" customHeight="1">
+    <row r="5" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="75" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1">
+      <c r="B5" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="76" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="38" hidden="1" customHeight="1" thickTop="1"/>
-    <row r="8" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="9" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="10" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="11" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="12" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="13" spans="1:2" ht="38" hidden="1" customHeight="1">
+      <c r="B6" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="38.1" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -1380,86 +3334,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="21" customWidth="1"/>
     <col min="6" max="6" width="34.5" style="21" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="15" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
       <c r="G1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:8" ht="39" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="H1" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="1:8" ht="39" customHeight="1">
-      <c r="A3" s="44" t="s">
+      <c r="H2" s="24">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
-    </row>
-    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1">
-      <c r="A4" s="46" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="40">
+        <v>34</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+    </row>
+    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
-    </row>
-    <row r="5" spans="1:8" ht="26" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1">
+      <c r="B4" s="52"/>
+      <c r="C4" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
+    </row>
+    <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1475,955 +3441,1075 @@
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-    </row>
-    <row r="7" spans="1:8" ht="39" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
+    </row>
+    <row r="7" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
-    </row>
-    <row r="8" spans="1:8" ht="39" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="F7" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" ht="39" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="F8" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="23"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
-    </row>
-    <row r="10" spans="1:8" ht="39" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="F9" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="23"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" ht="39" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="F10" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" ht="39" customHeight="1">
+      <c r="F11" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" ht="39" customHeight="1">
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" ht="39" customHeight="1">
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="30"/>
-    </row>
-    <row r="15" spans="1:8" ht="39" customHeight="1">
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+    </row>
+    <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" ht="39" customHeight="1">
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
-    </row>
-    <row r="17" spans="1:8" ht="39" customHeight="1">
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
+    </row>
+    <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="1:8" ht="39" customHeight="1">
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38"/>
+    </row>
+    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="30"/>
-    </row>
-    <row r="19" spans="1:8" ht="39" customHeight="1">
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+    </row>
+    <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
-    </row>
-    <row r="20" spans="1:8" ht="39" customHeight="1">
+      <c r="F19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
+    </row>
+    <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="30"/>
-    </row>
-    <row r="21" spans="1:8" ht="39" customHeight="1">
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
+    </row>
+    <row r="21" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="30"/>
-    </row>
-    <row r="22" spans="1:8" ht="39" customHeight="1">
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="30"/>
-    </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1">
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+    </row>
+    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="30"/>
-    </row>
-    <row r="24" spans="1:8" ht="39" customHeight="1">
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
+    </row>
+    <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="23"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="30"/>
-    </row>
-    <row r="25" spans="1:8" ht="39" customHeight="1">
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="38"/>
+    </row>
+    <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
       <c r="E25" s="23"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
-    </row>
-    <row r="26" spans="1:8" ht="39" customHeight="1">
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="23"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-    </row>
-    <row r="27" spans="1:8" ht="39" customHeight="1">
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="5"/>
       <c r="E27" s="23"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-    </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1">
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="5"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
-    </row>
-    <row r="29" spans="1:8" ht="39" customHeight="1">
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-    </row>
-    <row r="30" spans="1:8" ht="39" customHeight="1">
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30"/>
-    </row>
-    <row r="31" spans="1:8" ht="39" customHeight="1">
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
+    </row>
+    <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="30"/>
-    </row>
-    <row r="32" spans="1:8" ht="39" customHeight="1">
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
+    </row>
+    <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="30"/>
-    </row>
-    <row r="33" spans="1:8" ht="39" customHeight="1">
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
+    </row>
+    <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
       <c r="E33" s="23"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="30"/>
-    </row>
-    <row r="34" spans="1:8" ht="39" customHeight="1">
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
+    </row>
+    <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5"/>
       <c r="E34" s="23"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="30"/>
-    </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1">
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="5"/>
       <c r="E35" s="23"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="30"/>
-    </row>
-    <row r="36" spans="1:8" ht="39" customHeight="1">
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="38"/>
+    </row>
+    <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="30"/>
-    </row>
-    <row r="37" spans="1:8" ht="39" customHeight="1">
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
+    </row>
+    <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="5"/>
       <c r="E37" s="23"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
-    </row>
-    <row r="38" spans="1:8" ht="39" customHeight="1">
+      <c r="F37" s="36"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="38"/>
+    </row>
+    <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="5"/>
       <c r="E38" s="23"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="30"/>
-    </row>
-    <row r="39" spans="1:8" ht="39" customHeight="1">
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="38"/>
+    </row>
+    <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="5"/>
       <c r="E39" s="23"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="30"/>
-    </row>
-    <row r="40" spans="1:8" ht="39" customHeight="1">
+      <c r="F39" s="36"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="38"/>
+    </row>
+    <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="5"/>
       <c r="E40" s="23"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="30"/>
-    </row>
-    <row r="41" spans="1:8" ht="39" customHeight="1">
+      <c r="F40" s="36"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+    </row>
+    <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="5"/>
       <c r="E41" s="23"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="30"/>
-    </row>
-    <row r="42" spans="1:8" ht="39" customHeight="1">
+      <c r="F41" s="36"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="38"/>
+    </row>
+    <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="23"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="30"/>
-    </row>
-    <row r="43" spans="1:8" ht="39" customHeight="1">
+      <c r="F42" s="36"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="38"/>
+    </row>
+    <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="5"/>
       <c r="E43" s="23"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="30"/>
-    </row>
-    <row r="44" spans="1:8" ht="39" customHeight="1">
+      <c r="F43" s="36"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="38"/>
+    </row>
+    <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="23"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="30"/>
-    </row>
-    <row r="45" spans="1:8" ht="39" customHeight="1">
+      <c r="F44" s="36"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38"/>
+    </row>
+    <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>
       <c r="E45" s="23"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="30"/>
-    </row>
-    <row r="46" spans="1:8" ht="39" customHeight="1">
+      <c r="F45" s="36"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="38"/>
+    </row>
+    <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="23"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="30"/>
-    </row>
-    <row r="47" spans="1:8" ht="39" customHeight="1">
+      <c r="F46" s="36"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
+    </row>
+    <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="23"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="30"/>
-    </row>
-    <row r="48" spans="1:8" ht="39" customHeight="1">
+      <c r="F47" s="36"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="38"/>
+    </row>
+    <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
       <c r="E48" s="23"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="30"/>
-    </row>
-    <row r="49" spans="1:8" ht="39" customHeight="1">
+      <c r="F48" s="36"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="38"/>
+    </row>
+    <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
       <c r="E49" s="23"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="30"/>
-    </row>
-    <row r="50" spans="1:8" ht="39" customHeight="1">
+      <c r="F49" s="36"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="38"/>
+    </row>
+    <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="5"/>
       <c r="E50" s="23"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="30"/>
-    </row>
-    <row r="51" spans="1:8" ht="39" customHeight="1">
+      <c r="F50" s="36"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="38"/>
+    </row>
+    <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="5"/>
       <c r="E51" s="23"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="30"/>
-    </row>
-    <row r="52" spans="1:8" ht="39" customHeight="1">
+      <c r="F51" s="36"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="38"/>
+    </row>
+    <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="5"/>
       <c r="E52" s="23"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="30"/>
-    </row>
-    <row r="53" spans="1:8" ht="39" customHeight="1">
+      <c r="F52" s="36"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="38"/>
+    </row>
+    <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
       <c r="E53" s="23"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="30"/>
-    </row>
-    <row r="54" spans="1:8" ht="39" customHeight="1">
+      <c r="F53" s="36"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="38"/>
+    </row>
+    <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
       <c r="E54" s="23"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="30"/>
-    </row>
-    <row r="55" spans="1:8" ht="39" customHeight="1">
+      <c r="F54" s="36"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="38"/>
+    </row>
+    <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
       <c r="E55" s="23"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="30"/>
-    </row>
-    <row r="56" spans="1:8" ht="39" customHeight="1">
+      <c r="F55" s="36"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="38"/>
+    </row>
+    <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
       <c r="E56" s="23"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="30"/>
-    </row>
-    <row r="57" spans="1:8" ht="39" customHeight="1">
+      <c r="F56" s="36"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="38"/>
+    </row>
+    <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
       <c r="E57" s="23"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="30"/>
-    </row>
-    <row r="58" spans="1:8" ht="39" customHeight="1">
+      <c r="F57" s="36"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="38"/>
+    </row>
+    <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
       <c r="E58" s="23"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="30"/>
-    </row>
-    <row r="59" spans="1:8" ht="39" customHeight="1">
+      <c r="F58" s="36"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="38"/>
+    </row>
+    <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
       <c r="E59" s="23"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="29"/>
-      <c r="H59" s="30"/>
-    </row>
-    <row r="60" spans="1:8" ht="39" customHeight="1">
+      <c r="F59" s="36"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="38"/>
+    </row>
+    <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
       <c r="E60" s="23"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="30"/>
-    </row>
-    <row r="61" spans="1:8" ht="39" customHeight="1">
+      <c r="F60" s="36"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="38"/>
+    </row>
+    <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
       <c r="E61" s="23"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="30"/>
-    </row>
-    <row r="62" spans="1:8" ht="39" customHeight="1">
+      <c r="F61" s="36"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="38"/>
+    </row>
+    <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="23"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="30"/>
-    </row>
-    <row r="63" spans="1:8" ht="39" customHeight="1">
+      <c r="F62" s="36"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="38"/>
+    </row>
+    <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="23"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="30"/>
-    </row>
-    <row r="64" spans="1:8" ht="39" customHeight="1">
+      <c r="F63" s="36"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="38"/>
+    </row>
+    <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="30"/>
-    </row>
-    <row r="65" spans="1:8" ht="39" customHeight="1">
+      <c r="F64" s="36"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="38"/>
+    </row>
+    <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="23"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="30"/>
-    </row>
-    <row r="66" spans="1:8" ht="39" customHeight="1">
+      <c r="F65" s="36"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="38"/>
+    </row>
+    <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="23"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="30"/>
-    </row>
-    <row r="67" spans="1:8" ht="39" customHeight="1">
+      <c r="F66" s="36"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="38"/>
+    </row>
+    <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="23"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="30"/>
-    </row>
-    <row r="68" spans="1:8" ht="39" customHeight="1">
+      <c r="F67" s="36"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="38"/>
+    </row>
+    <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="23"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="30"/>
-    </row>
-    <row r="69" spans="1:8" ht="39" customHeight="1">
+      <c r="F68" s="36"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="38"/>
+    </row>
+    <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="23"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="30"/>
-    </row>
-    <row r="70" spans="1:8" ht="39" customHeight="1">
+      <c r="F69" s="36"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="38"/>
+    </row>
+    <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="23"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="30"/>
-    </row>
-    <row r="71" spans="1:8" ht="39" customHeight="1">
+      <c r="F70" s="36"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="38"/>
+    </row>
+    <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="23"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="30"/>
-    </row>
-    <row r="72" spans="1:8" ht="39" customHeight="1">
+      <c r="F71" s="36"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="38"/>
+    </row>
+    <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="23"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="30"/>
-    </row>
-    <row r="73" spans="1:8" ht="39" customHeight="1">
+      <c r="F72" s="36"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="38"/>
+    </row>
+    <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="23"/>
-      <c r="F73" s="28"/>
-      <c r="G73" s="29"/>
-      <c r="H73" s="30"/>
-    </row>
-    <row r="74" spans="1:8" ht="39" customHeight="1">
+      <c r="F73" s="36"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="38"/>
+    </row>
+    <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="23"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="29"/>
-      <c r="H74" s="30"/>
-    </row>
-    <row r="75" spans="1:8" ht="39" customHeight="1">
+      <c r="F74" s="36"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="38"/>
+    </row>
+    <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="23"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="29"/>
-      <c r="H75" s="30"/>
-    </row>
-    <row r="76" spans="1:8" ht="39" customHeight="1">
+      <c r="F75" s="36"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="38"/>
+    </row>
+    <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="23"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="29"/>
-      <c r="H76" s="30"/>
-    </row>
-    <row r="77" spans="1:8" ht="39" customHeight="1">
+      <c r="F76" s="36"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="38"/>
+    </row>
+    <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="23"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="30"/>
-    </row>
-    <row r="78" spans="1:8" ht="39" customHeight="1">
+      <c r="F77" s="36"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="38"/>
+    </row>
+    <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="23"/>
-      <c r="F78" s="28"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="30"/>
-    </row>
-    <row r="79" spans="1:8" ht="39" customHeight="1">
+      <c r="F78" s="36"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="38"/>
+    </row>
+    <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="23"/>
-      <c r="F79" s="28"/>
-      <c r="G79" s="29"/>
-      <c r="H79" s="30"/>
-    </row>
-    <row r="80" spans="1:8" ht="39" customHeight="1">
+      <c r="F79" s="36"/>
+      <c r="G79" s="37"/>
+      <c r="H79" s="38"/>
+    </row>
+    <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="23"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="29"/>
-      <c r="H80" s="30"/>
-    </row>
-    <row r="81" spans="1:8" ht="39" customHeight="1">
+      <c r="F80" s="36"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="38"/>
+    </row>
+    <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="23"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="29"/>
-      <c r="H81" s="30"/>
-    </row>
-    <row r="82" spans="1:8" ht="39" customHeight="1">
+      <c r="F81" s="36"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="38"/>
+    </row>
+    <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="23"/>
-      <c r="F82" s="28"/>
-      <c r="G82" s="29"/>
-      <c r="H82" s="30"/>
-    </row>
-    <row r="83" spans="1:8" ht="39" customHeight="1">
+      <c r="F82" s="36"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="38"/>
+    </row>
+    <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="23"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="29"/>
-      <c r="H83" s="30"/>
-    </row>
-    <row r="84" spans="1:8" ht="39" customHeight="1">
+      <c r="F83" s="36"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="38"/>
+    </row>
+    <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="23"/>
-      <c r="F84" s="28"/>
-      <c r="G84" s="29"/>
-      <c r="H84" s="30"/>
-    </row>
-    <row r="85" spans="1:8" ht="39" customHeight="1">
+      <c r="F84" s="36"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="38"/>
+    </row>
+    <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="23"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="30"/>
-    </row>
-    <row r="86" spans="1:8" ht="39" customHeight="1">
+      <c r="F85" s="36"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="38"/>
+    </row>
+    <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="23"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="29"/>
-      <c r="H86" s="30"/>
-    </row>
-    <row r="87" spans="1:8" ht="39" customHeight="1">
+      <c r="F86" s="36"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="38"/>
+    </row>
+    <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="23"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="30"/>
-    </row>
-    <row r="88" spans="1:8" ht="39" customHeight="1">
+      <c r="F87" s="36"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="38"/>
+    </row>
+    <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="23"/>
-      <c r="F88" s="28"/>
-      <c r="G88" s="29"/>
-      <c r="H88" s="30"/>
-    </row>
-    <row r="89" spans="1:8" ht="39" customHeight="1">
+      <c r="F88" s="36"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="38"/>
+    </row>
+    <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="23"/>
-      <c r="F89" s="28"/>
-      <c r="G89" s="29"/>
-      <c r="H89" s="30"/>
-    </row>
-    <row r="90" spans="1:8" ht="39" customHeight="1">
+      <c r="F89" s="36"/>
+      <c r="G89" s="37"/>
+      <c r="H89" s="38"/>
+    </row>
+    <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="23"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="30"/>
-    </row>
-    <row r="91" spans="1:8" ht="39" customHeight="1">
+      <c r="F90" s="36"/>
+      <c r="G90" s="37"/>
+      <c r="H90" s="38"/>
+    </row>
+    <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="23"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="29"/>
-      <c r="H91" s="30"/>
-    </row>
-    <row r="92" spans="1:8" ht="39" customHeight="1">
+      <c r="F91" s="36"/>
+      <c r="G91" s="37"/>
+      <c r="H91" s="38"/>
+    </row>
+    <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="23"/>
-      <c r="F92" s="28"/>
-      <c r="G92" s="29"/>
-      <c r="H92" s="30"/>
-    </row>
-    <row r="93" spans="1:8" ht="39" customHeight="1">
+      <c r="F92" s="36"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="38"/>
+    </row>
+    <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="23"/>
-      <c r="F93" s="28"/>
-      <c r="G93" s="29"/>
-      <c r="H93" s="30"/>
-    </row>
-    <row r="94" spans="1:8" ht="39" customHeight="1">
+      <c r="F93" s="36"/>
+      <c r="G93" s="37"/>
+      <c r="H93" s="38"/>
+    </row>
+    <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="23"/>
-      <c r="F94" s="28"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="30"/>
-    </row>
-    <row r="95" spans="1:8" ht="39" customHeight="1">
+      <c r="F94" s="36"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="38"/>
+    </row>
+    <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="30"/>
-    </row>
-    <row r="96" spans="1:8" ht="39" customHeight="1">
+      <c r="F95" s="36"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="38"/>
+    </row>
+    <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="23"/>
-      <c r="F96" s="28"/>
-      <c r="G96" s="29"/>
-      <c r="H96" s="30"/>
-    </row>
-    <row r="97" spans="1:8" ht="39" customHeight="1">
+      <c r="F96" s="36"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="38"/>
+    </row>
+    <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="23"/>
-      <c r="F97" s="28"/>
-      <c r="G97" s="29"/>
-      <c r="H97" s="30"/>
-    </row>
-    <row r="98" spans="1:8" ht="39" customHeight="1">
+      <c r="F97" s="36"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="38"/>
+    </row>
+    <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="23"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="29"/>
-      <c r="H98" s="30"/>
-    </row>
-    <row r="99" spans="1:8" ht="39" customHeight="1">
+      <c r="F98" s="36"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="38"/>
+    </row>
+    <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="23"/>
-      <c r="F99" s="28"/>
-      <c r="G99" s="29"/>
-      <c r="H99" s="30"/>
-    </row>
-    <row r="100" spans="1:8" ht="39" customHeight="1">
+      <c r="F99" s="36"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="38"/>
+    </row>
+    <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="23"/>
-      <c r="F100" s="28"/>
-      <c r="G100" s="29"/>
-      <c r="H100" s="30"/>
-    </row>
-    <row r="101" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1"/>
+      <c r="F100" s="36"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="38"/>
+    </row>
+    <row r="101" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -2438,100 +4524,10 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -2544,93 +4540,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="21.875" style="17" customWidth="1"/>
     <col min="2" max="4" width="15" style="17" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="17" customWidth="1"/>
     <col min="6" max="16384" width="15" style="17" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1">
+    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
-    </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="56"/>
+    </row>
+    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
-    </row>
-    <row r="3" spans="1:5" ht="136" customHeight="1">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="58"/>
+    </row>
+    <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-    </row>
-    <row r="4" spans="1:5" ht="46" customHeight="1">
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="60"/>
+    </row>
+    <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-    </row>
-    <row r="5" spans="1:5" ht="46" customHeight="1">
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65"/>
+    </row>
+    <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="55"/>
-    </row>
-    <row r="6" spans="1:5" ht="46" customHeight="1">
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="60"/>
+    </row>
+    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-    </row>
-    <row r="7" spans="1:5" ht="46" customHeight="1">
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
+    </row>
+    <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="60"/>
-    </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1">
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
+    </row>
+    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2645,7 +4641,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -2658,215 +4654,215 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2" hidden="1"/>
+    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="10.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="63"/>
-    </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1">
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
+    </row>
+    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="77">
+      <c r="B2" s="69">
         <v>41806</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="55"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
-    </row>
-    <row r="4" spans="1:7" ht="112" customHeight="1">
+      <c r="B3" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="60"/>
+    </row>
+    <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55"/>
-    </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1">
+      <c r="B4" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="60"/>
+    </row>
+    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
-    </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
-    <row r="7" spans="1:7" ht="36" customHeight="1">
-      <c r="A7" s="61" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
+    </row>
+    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63"/>
-    </row>
-    <row r="8" spans="1:7" ht="36" customHeight="1">
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="68"/>
+    </row>
+    <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="69"/>
-    </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1">
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="71"/>
+    </row>
+    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
-    </row>
-    <row r="10" spans="1:7" ht="112" customHeight="1">
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
+    </row>
+    <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1">
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
+    </row>
+    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="71"/>
-    </row>
-    <row r="12" spans="1:7" ht="36" customHeight="1"/>
-    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
-    <row r="14" spans="1:7" ht="36" customHeight="1">
-      <c r="A14" s="61" t="s">
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="73"/>
+    </row>
+    <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="63"/>
-    </row>
-    <row r="15" spans="1:7" ht="36" customHeight="1">
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="68"/>
+    </row>
+    <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65"/>
-    </row>
-    <row r="16" spans="1:7" ht="36" customHeight="1">
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="75"/>
+    </row>
+    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="55"/>
-    </row>
-    <row r="17" spans="1:7" ht="113" customHeight="1">
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+    </row>
+    <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
-    </row>
-    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1">
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+    </row>
+    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="67"/>
-    </row>
-    <row r="19" spans="1:7" ht="36" customHeight="1"/>
-    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="77"/>
+    </row>
+    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -2877,13 +4873,129 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-119.28594970703099</v>
+      </c>
+      <c r="B2">
+        <v>-8.1960477828979403</v>
+      </c>
+      <c r="E2">
+        <v>-119.276565551757</v>
+      </c>
+      <c r="F2">
+        <v>-4.2161784172058097</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-107.45529937744099</v>
+      </c>
+      <c r="B3">
+        <v>-6.9468455314636204</v>
+      </c>
+      <c r="E3">
+        <v>-107.4468460083</v>
+      </c>
+      <c r="F3">
+        <v>-2.84029865264892</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-95.554893493652301</v>
+      </c>
+      <c r="B4">
+        <v>-5.5849814414978001</v>
+      </c>
+      <c r="E4">
+        <v>-95.544990539550696</v>
+      </c>
+      <c r="F4">
+        <v>-2.1803574562072701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-83.666122436523395</v>
+      </c>
+      <c r="B5">
+        <v>-1.8713792562484699</v>
+      </c>
+      <c r="E5">
+        <v>-83.659782409667898</v>
+      </c>
+      <c r="F5">
+        <v>-1.0234618186950599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-71.812217712402301</v>
+      </c>
+      <c r="B6">
+        <v>-0.72266530990600597</v>
+      </c>
+      <c r="E6">
+        <v>-71.810638427734304</v>
+      </c>
+      <c r="F6">
+        <v>1.33055078983306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-59.924896240234297</v>
+      </c>
+      <c r="B7">
+        <v>4.64208555221557</v>
+      </c>
+      <c r="E7">
+        <v>-59.928199768066399</v>
+      </c>
+      <c r="F7">
+        <v>2.36196541786193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-48.044841766357401</v>
+      </c>
+      <c r="B8">
+        <v>9.7224264144897408</v>
+      </c>
+      <c r="E8">
+        <v>-48.055477142333899</v>
+      </c>
+      <c r="F8">
+        <v>5.7743024826049796</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>